<commit_message>
refactored MsgBox interactions to allow for non interactiveness fixed EditDBModifDef display when no active workbook visible visual aid for DBSheets
</commit_message>
<xml_diff>
--- a/test/DBSheetsTest.xlsx
+++ b/test/DBSheetsTest.xlsx
@@ -49,7 +49,7 @@
     <definedName name="DBFtarget992c0b939c834927b5b4be12e7c5f3bc" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget9dcfa89545974284a4e8215f57a7dc41" hidden="1">discounts!$B$1:$G$4</definedName>
     <definedName name="DBFtargetafaeef3da22240e7856064ff43f8d6d8" hidden="1">publishers!$B$1:$F$9</definedName>
-    <definedName name="DBFtargetb648a6b572ea4b258d6eddefa1f1a1a2" hidden="1">employee!$B$1:$J$49</definedName>
+    <definedName name="DBFtargetb648a6b572ea4b258d6eddefa1f1a1a2" hidden="1">employee!$B$1:$J$48</definedName>
     <definedName name="DBFtargetba58cf4be2a54e63af8d36a10a2307ca" hidden="1">jobs!$B$1:$E$15</definedName>
     <definedName name="DBFtargetbbf44909fbc248689a82885fda31d908" hidden="1">LStitles!$B$2:$C$9</definedName>
     <definedName name="DBFtargetd71aa659a0864d838c2b664cc128979b" hidden="1">LStitleauthor!$C$2:$D$18</definedName>
@@ -59,7 +59,7 @@
     <definedName name="DBFtargetf4ff6127b9e24ce29b99ad13e11762a6" hidden="1">LSemployee!$A$2:$B$15</definedName>
     <definedName name="DBMapperauthors">authors!$B$1:$J$24</definedName>
     <definedName name="DBMapperdiscounts">discounts!$B$1:$G$4</definedName>
-    <definedName name="DBMapperemployee">employee!$B$1:$J$49</definedName>
+    <definedName name="DBMapperemployee">employee!$B$1:$J$48</definedName>
     <definedName name="DBMapperjobs">jobs!$B$1:$E$15</definedName>
     <definedName name="DBMapperpublishers">publishers!$B$1:$F$9</definedName>
     <definedName name="DBMapperroysched">roysched!$B$1:$F$87</definedName>
@@ -67,7 +67,7 @@
     <definedName name="DBMappertitles">titles!$B$1:$L$18</definedName>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">authors!$B$1:$J$24</definedName>
     <definedName name="ExterneDaten_1" localSheetId="2" hidden="1">discounts!$B$1:$F$4</definedName>
-    <definedName name="ExterneDaten_1" localSheetId="4" hidden="1">employee!$B$1:$H$49</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="4" hidden="1">employee!$B$1:$H$48</definedName>
     <definedName name="ExterneDaten_1" localSheetId="5" hidden="1">jobs!$B$1:$E$15</definedName>
     <definedName name="ExterneDaten_1" localSheetId="6" hidden="1">publishers!$B$1:$F$9</definedName>
     <definedName name="ExterneDaten_1" localSheetId="8" hidden="1">roysched!$B$1:$E$87</definedName>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="526">
   <si>
     <t xml:space="preserve">SELECT T1.au_id, T1.au_lname, T1.au_fname, T1.phone, T1.address, T1.city, T1.state, T1.zip, T1.contract_x000D_
 FROM pubs.dbo.authors T1 _x000D_
@@ -816,9 +816,6 @@
   </si>
   <si>
     <t>Accorti</t>
-  </si>
-  <si>
-    <t>PMA42628M</t>
   </si>
   <si>
     <t>B</t>
@@ -1792,6 +1789,53 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1957,53 +2001,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -2986,33 +2983,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle_ExterneDaten_1" displayName="Tabelle_ExterneDaten_1" ref="B1:J24" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle_ExterneDaten_1" displayName="Tabelle_ExterneDaten_1" ref="B1:J24" tableType="queryTable" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="B1:J24"/>
   <tableColumns count="9">
-    <tableColumn id="6" uniqueName="6" name="au_id" queryTableFieldId="44" dataDxfId="10"/>
-    <tableColumn id="7" uniqueName="7" name="au_lname" queryTableFieldId="45" dataDxfId="9"/>
-    <tableColumn id="8" uniqueName="8" name="au_fname" queryTableFieldId="46" dataDxfId="8"/>
-    <tableColumn id="9" uniqueName="9" name="phone" queryTableFieldId="47" dataDxfId="7"/>
-    <tableColumn id="10" uniqueName="10" name="address" queryTableFieldId="48" dataDxfId="6"/>
-    <tableColumn id="11" uniqueName="11" name="city" queryTableFieldId="49" dataDxfId="5"/>
-    <tableColumn id="12" uniqueName="12" name="state" queryTableFieldId="50" dataDxfId="4"/>
-    <tableColumn id="13" uniqueName="13" name="zip" queryTableFieldId="51" dataDxfId="3"/>
-    <tableColumn id="14" uniqueName="14" name="contract" queryTableFieldId="52" dataDxfId="2"/>
+    <tableColumn id="6" uniqueName="6" name="au_id" queryTableFieldId="44" dataDxfId="70"/>
+    <tableColumn id="7" uniqueName="7" name="au_lname" queryTableFieldId="45" dataDxfId="69"/>
+    <tableColumn id="8" uniqueName="8" name="au_fname" queryTableFieldId="46" dataDxfId="68"/>
+    <tableColumn id="9" uniqueName="9" name="phone" queryTableFieldId="47" dataDxfId="67"/>
+    <tableColumn id="10" uniqueName="10" name="address" queryTableFieldId="48" dataDxfId="66"/>
+    <tableColumn id="11" uniqueName="11" name="city" queryTableFieldId="49" dataDxfId="65"/>
+    <tableColumn id="12" uniqueName="12" name="state" queryTableFieldId="50" dataDxfId="64"/>
+    <tableColumn id="13" uniqueName="13" name="zip" queryTableFieldId="51" dataDxfId="63"/>
+    <tableColumn id="14" uniqueName="14" name="contract" queryTableFieldId="52" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_ExterneDaten_13" displayName="Tabelle_ExterneDaten_13" ref="B1:G4" tableType="queryTable" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_ExterneDaten_13" displayName="Tabelle_ExterneDaten_13" ref="B1:G4" tableType="queryTable" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="B1:G4"/>
   <tableColumns count="6">
-    <tableColumn id="3" uniqueName="3" name="discounttype" queryTableFieldId="2" dataDxfId="70"/>
-    <tableColumn id="4" uniqueName="4" name="stor_idLU" queryTableFieldId="3" dataDxfId="69"/>
-    <tableColumn id="5" uniqueName="5" name="lowqty" queryTableFieldId="4" dataDxfId="68"/>
-    <tableColumn id="6" uniqueName="6" name="highqty" queryTableFieldId="5" dataDxfId="67"/>
-    <tableColumn id="7" uniqueName="7" name="discount" queryTableFieldId="6" dataDxfId="66"/>
-    <tableColumn id="8" uniqueName="8" name="stor_id" queryTableFieldId="7" dataDxfId="65">
+    <tableColumn id="3" uniqueName="3" name="discounttype" queryTableFieldId="2" dataDxfId="59"/>
+    <tableColumn id="4" uniqueName="4" name="stor_idLU" queryTableFieldId="3" dataDxfId="58"/>
+    <tableColumn id="5" uniqueName="5" name="lowqty" queryTableFieldId="4" dataDxfId="57"/>
+    <tableColumn id="6" uniqueName="6" name="highqty" queryTableFieldId="5" dataDxfId="56"/>
+    <tableColumn id="7" uniqueName="7" name="discount" queryTableFieldId="6" dataDxfId="55"/>
+    <tableColumn id="8" uniqueName="8" name="stor_id" queryTableFieldId="7" dataDxfId="54">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_13[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_13[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3021,20 +3018,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle_ExterneDaten_14" displayName="Tabelle_ExterneDaten_14" ref="B1:J49" tableType="queryTable" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="B1:J49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle_ExterneDaten_14" displayName="Tabelle_ExterneDaten_14" ref="B1:J48" tableType="queryTable" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="B1:J48"/>
   <tableColumns count="9">
-    <tableColumn id="3" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="62"/>
-    <tableColumn id="4" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="61"/>
-    <tableColumn id="5" uniqueName="5" name="minit" queryTableFieldId="4" dataDxfId="60"/>
-    <tableColumn id="6" uniqueName="6" name="lname" queryTableFieldId="5" dataDxfId="59"/>
-    <tableColumn id="7" uniqueName="7" name="job_idLU" queryTableFieldId="6" dataDxfId="58"/>
-    <tableColumn id="8" uniqueName="8" name="job_lvl" queryTableFieldId="7" dataDxfId="57"/>
-    <tableColumn id="9" uniqueName="9" name="pub_idLU" queryTableFieldId="8" dataDxfId="56"/>
-    <tableColumn id="10" uniqueName="10" name="job_id" queryTableFieldId="9" dataDxfId="55">
+    <tableColumn id="3" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="51"/>
+    <tableColumn id="4" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="50"/>
+    <tableColumn id="5" uniqueName="5" name="minit" queryTableFieldId="4" dataDxfId="49"/>
+    <tableColumn id="6" uniqueName="6" name="lname" queryTableFieldId="5" dataDxfId="48"/>
+    <tableColumn id="7" uniqueName="7" name="job_idLU" queryTableFieldId="6" dataDxfId="47"/>
+    <tableColumn id="8" uniqueName="8" name="job_lvl" queryTableFieldId="7" dataDxfId="46"/>
+    <tableColumn id="9" uniqueName="9" name="pub_idLU" queryTableFieldId="8" dataDxfId="45"/>
+    <tableColumn id="10" uniqueName="10" name="job_id" queryTableFieldId="9" dataDxfId="44">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" uniqueName="11" name="pub_id" queryTableFieldId="10" dataDxfId="54">
+    <tableColumn id="11" uniqueName="11" name="pub_id" queryTableFieldId="10" dataDxfId="43">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3043,41 +3040,41 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle_ExterneDaten_15" displayName="Tabelle_ExterneDaten_15" ref="B1:E15" tableType="queryTable" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle_ExterneDaten_15" displayName="Tabelle_ExterneDaten_15" ref="B1:E15" tableType="queryTable" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="B1:E15"/>
   <tableColumns count="4">
-    <tableColumn id="3" uniqueName="3" name="job_id" queryTableFieldId="2" dataDxfId="51"/>
-    <tableColumn id="4" uniqueName="4" name="job_desc" queryTableFieldId="3" dataDxfId="50"/>
-    <tableColumn id="5" uniqueName="5" name="min_lvl" queryTableFieldId="4" dataDxfId="49"/>
-    <tableColumn id="6" uniqueName="6" name="max_lvl" queryTableFieldId="5" dataDxfId="48"/>
+    <tableColumn id="3" uniqueName="3" name="job_id" queryTableFieldId="2" dataDxfId="40"/>
+    <tableColumn id="4" uniqueName="4" name="job_desc" queryTableFieldId="3" dataDxfId="39"/>
+    <tableColumn id="5" uniqueName="5" name="min_lvl" queryTableFieldId="4" dataDxfId="38"/>
+    <tableColumn id="6" uniqueName="6" name="max_lvl" queryTableFieldId="5" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle_ExterneDaten_16" displayName="Tabelle_ExterneDaten_16" ref="B1:F9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle_ExterneDaten_16" displayName="Tabelle_ExterneDaten_16" ref="B1:F9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="B1:F9"/>
   <tableColumns count="5">
-    <tableColumn id="3" uniqueName="3" name="pub_id" queryTableFieldId="2" dataDxfId="45"/>
-    <tableColumn id="4" uniqueName="4" name="pub_name" queryTableFieldId="3" dataDxfId="44"/>
-    <tableColumn id="5" uniqueName="5" name="city" queryTableFieldId="4" dataDxfId="43"/>
-    <tableColumn id="6" uniqueName="6" name="state" queryTableFieldId="5" dataDxfId="42"/>
-    <tableColumn id="7" uniqueName="7" name="country" queryTableFieldId="6" dataDxfId="41"/>
+    <tableColumn id="3" uniqueName="3" name="pub_id" queryTableFieldId="2" dataDxfId="34"/>
+    <tableColumn id="4" uniqueName="4" name="pub_name" queryTableFieldId="3" dataDxfId="33"/>
+    <tableColumn id="5" uniqueName="5" name="city" queryTableFieldId="4" dataDxfId="32"/>
+    <tableColumn id="6" uniqueName="6" name="state" queryTableFieldId="5" dataDxfId="31"/>
+    <tableColumn id="7" uniqueName="7" name="country" queryTableFieldId="6" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle_ExterneDaten_17" displayName="Tabelle_ExterneDaten_17" ref="B1:F87" tableType="queryTable" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle_ExterneDaten_17" displayName="Tabelle_ExterneDaten_17" ref="B1:F87" tableType="queryTable" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B1:F87"/>
   <tableColumns count="5">
-    <tableColumn id="3" uniqueName="3" name="title_idLU" queryTableFieldId="2" dataDxfId="38"/>
-    <tableColumn id="4" uniqueName="4" name="lorange" queryTableFieldId="3" dataDxfId="37"/>
-    <tableColumn id="5" uniqueName="5" name="hirange" queryTableFieldId="4" dataDxfId="36"/>
-    <tableColumn id="6" uniqueName="6" name="royalty" queryTableFieldId="5" dataDxfId="35"/>
-    <tableColumn id="7" uniqueName="7" name="title_id" queryTableFieldId="6" dataDxfId="34">
+    <tableColumn id="3" uniqueName="3" name="title_idLU" queryTableFieldId="2" dataDxfId="27"/>
+    <tableColumn id="4" uniqueName="4" name="lorange" queryTableFieldId="3" dataDxfId="26"/>
+    <tableColumn id="5" uniqueName="5" name="hirange" queryTableFieldId="4" dataDxfId="25"/>
+    <tableColumn id="6" uniqueName="6" name="royalty" queryTableFieldId="5" dataDxfId="24"/>
+    <tableColumn id="7" uniqueName="7" name="title_id" queryTableFieldId="6" dataDxfId="23">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_17[[#This Row],[title_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_17[[#This Row],[title_idLU]],title_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3086,17 +3083,17 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle_ExterneDaten_18" displayName="Tabelle_ExterneDaten_18" ref="B1:G26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle_ExterneDaten_18" displayName="Tabelle_ExterneDaten_18" ref="B1:G26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B1:G26"/>
   <tableColumns count="6">
-    <tableColumn id="3" uniqueName="3" name="au_idLU" queryTableFieldId="2" dataDxfId="31"/>
-    <tableColumn id="4" uniqueName="4" name="title_idLU" queryTableFieldId="3" dataDxfId="30"/>
-    <tableColumn id="5" uniqueName="5" name="au_ord" queryTableFieldId="4" dataDxfId="29"/>
-    <tableColumn id="6" uniqueName="6" name="royaltyper" queryTableFieldId="5" dataDxfId="28"/>
-    <tableColumn id="7" uniqueName="7" name="au_id" queryTableFieldId="6" dataDxfId="27">
+    <tableColumn id="3" uniqueName="3" name="au_idLU" queryTableFieldId="2" dataDxfId="20"/>
+    <tableColumn id="4" uniqueName="4" name="title_idLU" queryTableFieldId="3" dataDxfId="19"/>
+    <tableColumn id="5" uniqueName="5" name="au_ord" queryTableFieldId="4" dataDxfId="18"/>
+    <tableColumn id="6" uniqueName="6" name="royaltyper" queryTableFieldId="5" dataDxfId="17"/>
+    <tableColumn id="7" uniqueName="7" name="au_id" queryTableFieldId="6" dataDxfId="16">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_18[[#This Row],[au_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_18[[#This Row],[au_idLU]],au_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" uniqueName="8" name="title_id" queryTableFieldId="7" dataDxfId="26">
+    <tableColumn id="8" uniqueName="8" name="title_id" queryTableFieldId="7" dataDxfId="15">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_18[[#This Row],[title_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_18[[#This Row],[title_idLU]],title_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3105,20 +3102,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle_ExterneDaten_19" displayName="Tabelle_ExterneDaten_19" ref="B1:L18" tableType="queryTable" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle_ExterneDaten_19" displayName="Tabelle_ExterneDaten_19" ref="B1:L18" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="B1:L18"/>
   <tableColumns count="11">
-    <tableColumn id="3" uniqueName="3" name="title_id" queryTableFieldId="2" dataDxfId="23"/>
-    <tableColumn id="4" uniqueName="4" name="title" queryTableFieldId="3" dataDxfId="22"/>
-    <tableColumn id="5" uniqueName="5" name="type" queryTableFieldId="4" dataDxfId="21"/>
-    <tableColumn id="6" uniqueName="6" name="pub_idLU" queryTableFieldId="5" dataDxfId="20"/>
-    <tableColumn id="7" uniqueName="7" name="price" queryTableFieldId="6" dataDxfId="19"/>
-    <tableColumn id="8" uniqueName="8" name="advance" queryTableFieldId="7" dataDxfId="18"/>
-    <tableColumn id="9" uniqueName="9" name="royalty" queryTableFieldId="8" dataDxfId="17"/>
-    <tableColumn id="10" uniqueName="10" name="ytd_sales" queryTableFieldId="9" dataDxfId="16"/>
-    <tableColumn id="11" uniqueName="11" name="notes" queryTableFieldId="10" dataDxfId="15"/>
-    <tableColumn id="12" uniqueName="12" name="pubdate" queryTableFieldId="11" dataDxfId="14"/>
-    <tableColumn id="13" uniqueName="13" name="pub_id" queryTableFieldId="12" dataDxfId="13">
+    <tableColumn id="3" uniqueName="3" name="title_id" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="4" uniqueName="4" name="title" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="5" uniqueName="5" name="type" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="6" uniqueName="6" name="pub_idLU" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="7" uniqueName="7" name="price" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="8" uniqueName="8" name="advance" queryTableFieldId="7" dataDxfId="7"/>
+    <tableColumn id="9" uniqueName="9" name="royalty" queryTableFieldId="8" dataDxfId="6"/>
+    <tableColumn id="10" uniqueName="10" name="ytd_sales" queryTableFieldId="9" dataDxfId="5"/>
+    <tableColumn id="11" uniqueName="11" name="notes" queryTableFieldId="10" dataDxfId="4"/>
+    <tableColumn id="12" uniqueName="12" name="pubdate" queryTableFieldId="11" dataDxfId="3"/>
+    <tableColumn id="13" uniqueName="13" name="pub_id" queryTableFieldId="12" dataDxfId="2">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_19[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_19[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3401,15 +3398,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -3533,7 +3525,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -4180,257 +4172,257 @@
         <v>Env:Test, (last result:)Retrieved 23 records from: SELECT T1.au_lname + ' ' + T1.au_fname au_id,T1.au_id FROM pubs.dbo.authors T1 ORDER BY T1.au_lname</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C1" t="str">
         <f>_xll.DBListFetch(D1,"",title_idLookup)</f>
         <v>Env:Test, (last result:)Retrieved 17 records from: SELECT title,title_id FROM pubs.dbo.titles ORDER BY title</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B3" t="s">
         <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B5" t="s">
         <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B6" t="s">
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B9" t="s">
         <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B11" t="s">
         <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B12" t="s">
         <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B13" t="s">
         <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B14" t="s">
         <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B15" t="s">
         <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B17" t="s">
         <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B18" t="s">
         <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B19" t="s">
         <v>151</v>
@@ -4438,7 +4430,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
@@ -4446,7 +4438,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
@@ -4454,7 +4446,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B22" t="s">
         <v>117</v>
@@ -4462,7 +4454,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -4470,7 +4462,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B24" t="s">
         <v>94</v>
@@ -4508,33 +4500,33 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -4553,10 +4545,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -4575,10 +4567,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -4597,10 +4589,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -4619,10 +4611,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -4641,10 +4633,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -4663,10 +4655,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -4685,10 +4677,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -4707,10 +4699,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -4729,10 +4721,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -4751,10 +4743,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -4773,10 +4765,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -4795,10 +4787,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -4817,10 +4809,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -4839,10 +4831,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -4861,10 +4853,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -4883,10 +4875,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -4905,10 +4897,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
@@ -4927,10 +4919,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -4949,10 +4941,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -4971,10 +4963,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -4993,10 +4985,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D23" s="2">
         <v>2</v>
@@ -5015,10 +5007,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
@@ -5037,10 +5029,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -5059,10 +5051,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -5109,12 +5101,12 @@
         <v>Env:Test, (last result:)Retrieved 8 records from: SELECT pub_name,pub_id FROM pubs.dbo.publishers ORDER BY pub_name</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B2" t="s">
         <v>214</v>
@@ -5125,7 +5117,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B3" t="s">
         <v>212</v>
@@ -5136,7 +5128,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B4" t="s">
         <v>210</v>
@@ -5147,7 +5139,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B5" t="s">
         <v>208</v>
@@ -5158,7 +5150,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B6" t="s">
         <v>206</v>
@@ -5229,51 +5221,51 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>492</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>222</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>497</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>214</v>
@@ -5291,7 +5283,7 @@
         <v>4095</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K2" s="4">
         <v>33401</v>
@@ -5303,13 +5295,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>214</v>
@@ -5327,7 +5319,7 @@
         <v>3876</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K3" s="4">
         <v>33398</v>
@@ -5339,13 +5331,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>204</v>
@@ -5363,7 +5355,7 @@
         <v>18722</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K4" s="4">
         <v>33419</v>
@@ -5375,13 +5367,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>214</v>
@@ -5399,7 +5391,7 @@
         <v>4095</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K5" s="4">
         <v>33411</v>
@@ -5411,13 +5403,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>212</v>
@@ -5435,7 +5427,7 @@
         <v>2032</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K6" s="4">
         <v>33398</v>
@@ -5447,13 +5439,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>212</v>
@@ -5471,7 +5463,7 @@
         <v>22246</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K7" s="4">
         <v>33407</v>
@@ -5483,13 +5475,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>214</v>
@@ -5507,7 +5499,7 @@
         <v>8780</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K8" s="4">
         <v>33419</v>
@@ -5519,13 +5511,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>214</v>
@@ -5543,7 +5535,7 @@
         <v>4095</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K9" s="4">
         <v>34497</v>
@@ -5555,13 +5547,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>214</v>
@@ -5573,7 +5565,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K10" s="4">
         <v>43675.388807870368</v>
@@ -5585,13 +5577,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>212</v>
@@ -5609,7 +5601,7 @@
         <v>375</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K11" s="4">
         <v>33532</v>
@@ -5621,13 +5613,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>204</v>
@@ -5645,7 +5637,7 @@
         <v>2045</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K12" s="4">
         <v>33404</v>
@@ -5657,13 +5649,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>204</v>
@@ -5681,7 +5673,7 @@
         <v>111</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K13" s="4">
         <v>33516</v>
@@ -5693,13 +5685,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>204</v>
@@ -5717,7 +5709,7 @@
         <v>4072</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K14" s="4">
         <v>33401</v>
@@ -5729,13 +5721,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>204</v>
@@ -5753,7 +5745,7 @@
         <v>3336</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K15" s="4">
         <v>33401</v>
@@ -5765,13 +5757,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>212</v>
@@ -5789,7 +5781,7 @@
         <v>375</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K16" s="4">
         <v>33532</v>
@@ -5801,13 +5793,13 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>212</v>
@@ -5825,7 +5817,7 @@
         <v>15096</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K17" s="4">
         <v>33401</v>
@@ -5837,13 +5829,13 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>212</v>
@@ -5861,7 +5853,7 @@
         <v>4095</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K18" s="4">
         <v>33401</v>
@@ -6184,7 +6176,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -6213,7 +6205,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6262,10 +6254,10 @@
         <v>222</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6304,91 +6296,91 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G3" s="2">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I3" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G4" s="2">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I4" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J4" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>235</v>
+        <v>516</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G5" s="2">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I5" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6397,29 +6389,29 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>517</v>
+        <v>241</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="2">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I6" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J6" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6428,60 +6420,60 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>242</v>
+        <v>517</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G7" s="2">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I7" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J7" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>9952</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>518</v>
+        <v>248</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G8" s="2">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>200</v>
       </c>
       <c r="I8" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J8" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6490,112 +6482,112 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G9" s="2">
-        <v>215</v>
+        <v>87</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="I9" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J9" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9952</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>252</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G10" s="2">
-        <v>87</v>
+        <v>200</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="I10" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J10" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9952</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>254</v>
+        <v>518</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>519</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>256</v>
+        <v>520</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G11" s="2">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="I11" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="J11" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9952</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>519</v>
+        <v>258</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>520</v>
+        <v>259</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>521</v>
+        <v>261</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G12" s="2">
         <v>77</v>
@@ -6605,7 +6597,7 @@
       </c>
       <c r="I12" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6614,29 +6606,29 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G13" s="2">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I13" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J13" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6645,25 +6637,25 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>188</v>
       </c>
       <c r="G14" s="2">
-        <v>159</v>
+        <v>211</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I14" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -6671,61 +6663,61 @@
       </c>
       <c r="J14" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G15" s="2">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I15" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J15" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>273</v>
+        <v>521</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>193</v>
       </c>
       <c r="G16" s="2">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I16" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -6733,96 +6725,96 @@
       </c>
       <c r="J16" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>522</v>
+        <v>279</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="G17" s="2">
         <v>170</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I17" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J17" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G18" s="2">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I18" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J18" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G19" s="2">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>204</v>
       </c>
       <c r="I19" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J19" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6831,122 +6823,120 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G20" s="2">
-        <v>220</v>
+        <v>80</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I20" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J20" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G21" s="2">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I21" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J21" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>9901</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>295</v>
+        <v>241</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G22" s="2">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="I22" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J22" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9901</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>242</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G23" s="2">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>214</v>
       </c>
       <c r="I23" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J23" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -6955,107 +6945,107 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>303</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="E24" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G24" s="2">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I24" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J24" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>225</v>
+        <v>307</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G25" s="2">
-        <v>175</v>
+        <v>77</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I25" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="J25" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G26" s="2">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I26" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J26" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>312</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>191</v>
@@ -7064,7 +7054,7 @@
         <v>150</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I27" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -7072,156 +7062,158 @@
       </c>
       <c r="J27" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D28" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="E28" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G28" s="2">
-        <v>150</v>
+        <v>198</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="I28" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J28" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G29" s="2">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I29" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J29" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1622</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>321</v>
+        <v>522</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G30" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I30" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J30" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>523</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>235</v>
+        <v>326</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G31" s="2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I31" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J31" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>327</v>
+        <v>225</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G32" s="2">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>214</v>
       </c>
       <c r="I32" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J32" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7230,29 +7222,29 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G33" s="2">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>214</v>
       </c>
       <c r="I33" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J33" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7261,25 +7253,23 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>231</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>189</v>
       </c>
       <c r="G34" s="2">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I34" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -7287,94 +7277,94 @@
       </c>
       <c r="J34" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>297</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G35" s="2">
-        <v>101</v>
+        <v>246</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I35" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J35" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>280</v>
+        <v>341</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>339</v>
+        <v>188</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G36" s="2">
-        <v>246</v>
+        <v>100</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="I36" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J36" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1756</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>342</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>188</v>
+        <v>344</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="G37" s="2">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I37" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J37" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7383,54 +7373,54 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="D38" s="2"/>
+        <v>346</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>347</v>
+      </c>
       <c r="E38" s="2" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G38" s="2">
-        <v>77</v>
+        <v>192</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I38" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J38" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>348</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>194</v>
       </c>
       <c r="G39" s="2">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I39" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -7438,123 +7428,125 @@
       </c>
       <c r="J39" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G40" s="2">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="I40" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J40" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="E41" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G41" s="2">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I41" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J41" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G42" s="2">
-        <v>175</v>
+        <v>77</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I42" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J42" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>287</v>
+        <v>225</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="G43" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>214</v>
       </c>
       <c r="I43" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J43" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7563,60 +7555,60 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>225</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G44" s="2">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I44" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J44" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>225</v>
+        <v>268</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G45" s="2">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>204</v>
       </c>
       <c r="I45" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J45" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7625,134 +7617,103 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>367</v>
+        <v>256</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>368</v>
+        <v>523</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>269</v>
+        <v>227</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>369</v>
+        <v>524</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G46" s="2">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I46" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J46" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>257</v>
+        <v>369</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>524</v>
+        <v>114</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>525</v>
+        <v>370</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="G47" s="2">
-        <v>77</v>
+        <v>170</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I47" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J47" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>114</v>
+        <v>372</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G48" s="2">
-        <v>170</v>
+        <v>77</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I48" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J48" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G49" s="2">
-        <v>77</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="I49" s="2">
-        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
-      </c>
-      <c r="J49" s="2" t="str">
-        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
         <v>0877</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F48">
       <formula1>OFFSET(job_idLookup,0,0,,1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H48">
       <formula1>OFFSET(pub_idLookup,0,0,,1)</formula1>
     </dataValidation>
   </dataValidations>
@@ -7767,7 +7728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7787,21 +7750,21 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -7821,7 +7784,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
@@ -7992,7 +7955,7 @@
         <v>196</v>
       </c>
       <c r="D15" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2">
         <v>100</v>
@@ -8031,10 +7994,10 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -8043,12 +8006,12 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>205</v>
@@ -8057,13 +8020,13 @@
         <v>204</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8074,13 +8037,13 @@
         <v>212</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>388</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8097,7 +8060,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8108,13 +8071,13 @@
         <v>210</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8125,13 +8088,13 @@
         <v>202</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8142,11 +8105,11 @@
         <v>208</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8157,13 +8120,13 @@
         <v>200</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8174,11 +8137,11 @@
         <v>206</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -8203,7 +8166,7 @@
         <v>Env:Test, (last result:)Retrieved 17 records from: SELECT T1.title+'/'+p.pub_name AS title_id,T1.title_id FROM pubs.dbo.titles T1 LEFT JOIN pubs.dbo.publishers p ON T1.pub_id = p.pub_id ORDER BY T1.title</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -8239,27 +8202,27 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -8281,7 +8244,7 @@
         <v xml:space="preserve">WHERE T1.lorange &gt;  and T1.hirange &lt; </v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C3" s="2">
         <v>5001</v>
@@ -8299,7 +8262,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -8317,7 +8280,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C5" s="2">
         <v>2001</v>
@@ -8335,7 +8298,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C6" s="2">
         <v>3001</v>
@@ -8353,7 +8316,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C7" s="2">
         <v>4001</v>
@@ -8371,7 +8334,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C8" s="2">
         <v>10001</v>
@@ -8389,7 +8352,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -8407,7 +8370,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C10" s="2">
         <v>1001</v>
@@ -8425,7 +8388,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C11" s="2">
         <v>3001</v>
@@ -8443,7 +8406,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C12" s="2">
         <v>5001</v>
@@ -8461,7 +8424,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C13" s="2">
         <v>7001</v>
@@ -8479,7 +8442,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C14" s="2">
         <v>10001</v>
@@ -8497,7 +8460,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C15" s="2">
         <v>12001</v>
@@ -8515,7 +8478,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C16" s="2">
         <v>14001</v>
@@ -8533,7 +8496,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -8551,7 +8514,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C18" s="2">
         <v>1001</v>
@@ -8569,7 +8532,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C19" s="2">
         <v>5001</v>
@@ -8587,7 +8550,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C20" s="2">
         <v>10001</v>
@@ -8605,7 +8568,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -8623,7 +8586,7 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C22" s="2">
         <v>2001</v>
@@ -8641,7 +8604,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C23" s="2">
         <v>5001</v>
@@ -8659,7 +8622,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C24" s="2">
         <v>10001</v>
@@ -8677,7 +8640,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -8695,7 +8658,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C26" s="2">
         <v>1001</v>
@@ -8713,7 +8676,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C27" s="2">
         <v>2001</v>
@@ -8731,7 +8694,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C28" s="2">
         <v>4001</v>
@@ -8749,7 +8712,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C29" s="2">
         <v>6001</v>
@@ -8767,7 +8730,7 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C30" s="2">
         <v>8001</v>
@@ -8785,7 +8748,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C31" s="2">
         <v>10001</v>
@@ -8803,7 +8766,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C32" s="2">
         <v>12001</v>
@@ -8821,7 +8784,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -8839,7 +8802,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C34" s="2">
         <v>2001</v>
@@ -8857,7 +8820,7 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C35" s="2">
         <v>4001</v>
@@ -8875,7 +8838,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C36" s="2">
         <v>6001</v>
@@ -8893,7 +8856,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C37" s="2">
         <v>8001</v>
@@ -8911,7 +8874,7 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C38" s="2">
         <v>10001</v>
@@ -8929,7 +8892,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C39" s="2">
         <v>12001</v>
@@ -8947,7 +8910,7 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C40" s="2">
         <v>14001</v>
@@ -8965,7 +8928,7 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
@@ -8983,7 +8946,7 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C42" s="2">
         <v>5001</v>
@@ -9001,7 +8964,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C43" s="2">
         <v>10001</v>
@@ -9019,7 +8982,7 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C44" s="2">
         <v>15001</v>
@@ -9037,7 +9000,7 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
@@ -9055,7 +9018,7 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C46" s="2">
         <v>5001</v>
@@ -9073,7 +9036,7 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -9091,7 +9054,7 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C48" s="2">
         <v>5001</v>
@@ -9109,7 +9072,7 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C49" s="2">
         <v>10001</v>
@@ -9127,7 +9090,7 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C50" s="2">
         <v>15001</v>
@@ -9145,7 +9108,7 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -9163,7 +9126,7 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C52" s="2">
         <v>4001</v>
@@ -9181,7 +9144,7 @@
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C53" s="2">
         <v>8001</v>
@@ -9199,7 +9162,7 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C54" s="2">
         <v>12001</v>
@@ -9217,7 +9180,7 @@
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C55" s="2">
         <v>16001</v>
@@ -9235,7 +9198,7 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C56" s="2">
         <v>20001</v>
@@ -9253,7 +9216,7 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C57" s="2">
         <v>24001</v>
@@ -9271,7 +9234,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C58" s="2">
         <v>28001</v>
@@ -9289,7 +9252,7 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -9307,7 +9270,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C60" s="2">
         <v>2001</v>
@@ -9325,7 +9288,7 @@
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C61" s="2">
         <v>4001</v>
@@ -9343,7 +9306,7 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C62" s="2">
         <v>8001</v>
@@ -9361,7 +9324,7 @@
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C63" s="2">
         <v>12001</v>
@@ -9379,7 +9342,7 @@
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C64" s="2">
         <v>20001</v>
@@ -9397,7 +9360,7 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -9415,7 +9378,7 @@
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C66" s="2">
         <v>5001</v>
@@ -9433,7 +9396,7 @@
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C67" s="2">
         <v>15001</v>
@@ -9451,7 +9414,7 @@
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C68" s="2">
         <v>0</v>
@@ -9469,7 +9432,7 @@
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C69" s="2">
         <v>2001</v>
@@ -9487,7 +9450,7 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C70" s="2">
         <v>8001</v>
@@ -9505,7 +9468,7 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C71" s="2">
         <v>16001</v>
@@ -9523,7 +9486,7 @@
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C72" s="2">
         <v>24001</v>
@@ -9541,7 +9504,7 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C73" s="2">
         <v>32001</v>
@@ -9559,7 +9522,7 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C74" s="2">
         <v>40001</v>
@@ -9577,7 +9540,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -9595,7 +9558,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C76" s="2">
         <v>5001</v>
@@ -9613,7 +9576,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C77" s="2">
         <v>10001</v>
@@ -9631,7 +9594,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C78" s="2">
         <v>15001</v>
@@ -9649,7 +9612,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C79" s="2">
         <v>20001</v>
@@ -9667,7 +9630,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C80" s="2">
         <v>25001</v>
@@ -9685,7 +9648,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C81" s="2">
         <v>30001</v>
@@ -9703,7 +9666,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C82" s="2">
         <v>35001</v>
@@ -9721,7 +9684,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -9739,7 +9702,7 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C84" s="2">
         <v>10001</v>
@@ -9757,7 +9720,7 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C85" s="2">
         <v>20001</v>
@@ -9775,7 +9738,7 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C86" s="2">
         <v>30001</v>
@@ -9793,7 +9756,7 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C87" s="2">
         <v>40001</v>

</xml_diff>

<commit_message>
optionally pass noninteractive parameter to execDBModif (default = interactive) display excel data errors in errorMsg
</commit_message>
<xml_diff>
--- a/test/DBSheetsTest.xlsx
+++ b/test/DBSheetsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11310" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="authors" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="titles" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">publishers!$A$1:$A$2</definedName>
     <definedName name="au_idLookup">LStitleauthor!$A$2:$B$24</definedName>
     <definedName name="DBFsource008b1f5c6c9e4da4bb8c477f6a375b1a" hidden="1">LSdiscounts!$A$1</definedName>
     <definedName name="DBFsource048386b80dec4e9d87cf9513847ac5db" hidden="1">#REF!</definedName>
@@ -50,7 +51,7 @@
     <definedName name="DBFtarget9dcfa89545974284a4e8215f57a7dc41" hidden="1">discounts!$B$1:$G$4</definedName>
     <definedName name="DBFtargetafaeef3da22240e7856064ff43f8d6d8" hidden="1">publishers!$B$1:$F$9</definedName>
     <definedName name="DBFtargetb648a6b572ea4b258d6eddefa1f1a1a2" hidden="1">employee!$B$1:$J$48</definedName>
-    <definedName name="DBFtargetba58cf4be2a54e63af8d36a10a2307ca" hidden="1">jobs!$B$1:$E$15</definedName>
+    <definedName name="DBFtargetba58cf4be2a54e63af8d36a10a2307ca" hidden="1">jobs!$B$1:$E$16</definedName>
     <definedName name="DBFtargetbbf44909fbc248689a82885fda31d908" hidden="1">LStitles!$B$2:$C$9</definedName>
     <definedName name="DBFtargetd71aa659a0864d838c2b664cc128979b" hidden="1">LStitleauthor!$C$2:$D$18</definedName>
     <definedName name="DBFtargetd7f34f9f057d494fa071dbec688c6080" hidden="1">authors!$B$1:$J$24</definedName>
@@ -60,7 +61,7 @@
     <definedName name="DBMapperauthors">authors!$B$1:$J$24</definedName>
     <definedName name="DBMapperdiscounts">discounts!$B$1:$G$4</definedName>
     <definedName name="DBMapperemployee">employee!$B$1:$J$48</definedName>
-    <definedName name="DBMapperjobs">jobs!$B$1:$E$15</definedName>
+    <definedName name="DBMapperjobs">jobs!$B$1:$E$16</definedName>
     <definedName name="DBMapperpublishers">publishers!$B$1:$F$9</definedName>
     <definedName name="DBMapperroysched">roysched!$B$1:$F$87</definedName>
     <definedName name="DBMappertitleauthor">titleauthor!$B$1:$G$26</definedName>
@@ -68,7 +69,7 @@
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">authors!$B$1:$J$24</definedName>
     <definedName name="ExterneDaten_1" localSheetId="2" hidden="1">discounts!$B$1:$F$4</definedName>
     <definedName name="ExterneDaten_1" localSheetId="4" hidden="1">employee!$B$1:$H$48</definedName>
-    <definedName name="ExterneDaten_1" localSheetId="5" hidden="1">jobs!$B$1:$E$15</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="5" hidden="1">jobs!$B$1:$E$16</definedName>
     <definedName name="ExterneDaten_1" localSheetId="6" hidden="1">publishers!$B$1:$F$9</definedName>
     <definedName name="ExterneDaten_1" localSheetId="8" hidden="1">roysched!$B$1:$E$87</definedName>
     <definedName name="ExterneDaten_1" localSheetId="10" hidden="1">titleauthor!$B$1:$E$26</definedName>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="527">
   <si>
     <t xml:space="preserve">SELECT T1.au_id, T1.au_lname, T1.au_fname, T1.phone, T1.address, T1.city, T1.state, T1.zip, T1.contract_x000D_
 FROM pubs.dbo.authors T1 _x000D_
@@ -1729,6 +1730,9 @@
   </si>
   <si>
     <t>Muenchen</t>
+  </si>
+  <si>
+    <t>Acquisitions Manager2</t>
   </si>
 </sst>
 </file>
@@ -1789,53 +1793,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1926,6 +1883,53 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -2984,7 +2988,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle_ExterneDaten_1" displayName="Tabelle_ExterneDaten_1" ref="B1:J24" tableType="queryTable" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
-  <autoFilter ref="B1:J24"/>
   <tableColumns count="9">
     <tableColumn id="6" uniqueName="6" name="au_id" queryTableFieldId="44" dataDxfId="70"/>
     <tableColumn id="7" uniqueName="7" name="au_lname" queryTableFieldId="45" dataDxfId="69"/>
@@ -3002,7 +3005,6 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_ExterneDaten_13" displayName="Tabelle_ExterneDaten_13" ref="B1:G4" tableType="queryTable" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="B1:G4"/>
   <tableColumns count="6">
     <tableColumn id="3" uniqueName="3" name="discounttype" queryTableFieldId="2" dataDxfId="59"/>
     <tableColumn id="4" uniqueName="4" name="stor_idLU" queryTableFieldId="3" dataDxfId="58"/>
@@ -3019,7 +3021,6 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle_ExterneDaten_14" displayName="Tabelle_ExterneDaten_14" ref="B1:J48" tableType="queryTable" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="B1:J48"/>
   <tableColumns count="9">
     <tableColumn id="3" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="51"/>
     <tableColumn id="4" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="50"/>
@@ -3040,41 +3041,38 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle_ExterneDaten_15" displayName="Tabelle_ExterneDaten_15" ref="B1:E15" tableType="queryTable" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="B1:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle_ExterneDaten_15" displayName="Tabelle_ExterneDaten_15" ref="B1:E16" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <tableColumns count="4">
-    <tableColumn id="3" uniqueName="3" name="job_id" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="4" uniqueName="4" name="job_desc" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="5" uniqueName="5" name="min_lvl" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="6" uniqueName="6" name="max_lvl" queryTableFieldId="5" dataDxfId="37"/>
+    <tableColumn id="3" uniqueName="3" name="job_id" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="4" uniqueName="4" name="job_desc" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="5" uniqueName="5" name="min_lvl" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="6" uniqueName="6" name="max_lvl" queryTableFieldId="5" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle_ExterneDaten_16" displayName="Tabelle_ExterneDaten_16" ref="B1:F9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="B1:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle_ExterneDaten_16" displayName="Tabelle_ExterneDaten_16" ref="B1:F9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <tableColumns count="5">
-    <tableColumn id="3" uniqueName="3" name="pub_id" queryTableFieldId="2" dataDxfId="34"/>
-    <tableColumn id="4" uniqueName="4" name="pub_name" queryTableFieldId="3" dataDxfId="33"/>
-    <tableColumn id="5" uniqueName="5" name="city" queryTableFieldId="4" dataDxfId="32"/>
-    <tableColumn id="6" uniqueName="6" name="state" queryTableFieldId="5" dataDxfId="31"/>
-    <tableColumn id="7" uniqueName="7" name="country" queryTableFieldId="6" dataDxfId="30"/>
+    <tableColumn id="3" uniqueName="3" name="pub_id" queryTableFieldId="2" dataDxfId="40"/>
+    <tableColumn id="4" uniqueName="4" name="pub_name" queryTableFieldId="3" dataDxfId="39"/>
+    <tableColumn id="5" uniqueName="5" name="city" queryTableFieldId="4" dataDxfId="38"/>
+    <tableColumn id="6" uniqueName="6" name="state" queryTableFieldId="5" dataDxfId="37"/>
+    <tableColumn id="7" uniqueName="7" name="country" queryTableFieldId="6" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle_ExterneDaten_17" displayName="Tabelle_ExterneDaten_17" ref="B1:F87" tableType="queryTable" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="B1:F87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle_ExterneDaten_17" displayName="Tabelle_ExterneDaten_17" ref="B1:F87" tableType="queryTable" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <tableColumns count="5">
-    <tableColumn id="3" uniqueName="3" name="title_idLU" queryTableFieldId="2" dataDxfId="27"/>
-    <tableColumn id="4" uniqueName="4" name="lorange" queryTableFieldId="3" dataDxfId="26"/>
-    <tableColumn id="5" uniqueName="5" name="hirange" queryTableFieldId="4" dataDxfId="25"/>
-    <tableColumn id="6" uniqueName="6" name="royalty" queryTableFieldId="5" dataDxfId="24"/>
-    <tableColumn id="7" uniqueName="7" name="title_id" queryTableFieldId="6" dataDxfId="23">
+    <tableColumn id="3" uniqueName="3" name="title_idLU" queryTableFieldId="2" dataDxfId="33"/>
+    <tableColumn id="4" uniqueName="4" name="lorange" queryTableFieldId="3" dataDxfId="32"/>
+    <tableColumn id="5" uniqueName="5" name="hirange" queryTableFieldId="4" dataDxfId="31"/>
+    <tableColumn id="6" uniqueName="6" name="royalty" queryTableFieldId="5" dataDxfId="30"/>
+    <tableColumn id="7" uniqueName="7" name="title_id" queryTableFieldId="6" dataDxfId="29">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_17[[#This Row],[title_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_17[[#This Row],[title_idLU]],title_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3083,17 +3081,16 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle_ExterneDaten_18" displayName="Tabelle_ExterneDaten_18" ref="B1:G26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="B1:G26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle_ExterneDaten_18" displayName="Tabelle_ExterneDaten_18" ref="B1:G26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="6">
-    <tableColumn id="3" uniqueName="3" name="au_idLU" queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="4" uniqueName="4" name="title_idLU" queryTableFieldId="3" dataDxfId="19"/>
-    <tableColumn id="5" uniqueName="5" name="au_ord" queryTableFieldId="4" dataDxfId="18"/>
-    <tableColumn id="6" uniqueName="6" name="royaltyper" queryTableFieldId="5" dataDxfId="17"/>
-    <tableColumn id="7" uniqueName="7" name="au_id" queryTableFieldId="6" dataDxfId="16">
+    <tableColumn id="3" uniqueName="3" name="au_idLU" queryTableFieldId="2" dataDxfId="26"/>
+    <tableColumn id="4" uniqueName="4" name="title_idLU" queryTableFieldId="3" dataDxfId="25"/>
+    <tableColumn id="5" uniqueName="5" name="au_ord" queryTableFieldId="4" dataDxfId="24"/>
+    <tableColumn id="6" uniqueName="6" name="royaltyper" queryTableFieldId="5" dataDxfId="23"/>
+    <tableColumn id="7" uniqueName="7" name="au_id" queryTableFieldId="6" dataDxfId="22">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_18[[#This Row],[au_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_18[[#This Row],[au_idLU]],au_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" uniqueName="8" name="title_id" queryTableFieldId="7" dataDxfId="15">
+    <tableColumn id="8" uniqueName="8" name="title_id" queryTableFieldId="7" dataDxfId="21">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_18[[#This Row],[title_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_18[[#This Row],[title_idLU]],title_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3102,20 +3099,19 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle_ExterneDaten_19" displayName="Tabelle_ExterneDaten_19" ref="B1:L18" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="B1:L18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle_ExterneDaten_19" displayName="Tabelle_ExterneDaten_19" ref="B1:L18" tableType="queryTable" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="11">
-    <tableColumn id="3" uniqueName="3" name="title_id" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="4" uniqueName="4" name="title" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="5" uniqueName="5" name="type" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="6" uniqueName="6" name="pub_idLU" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="7" uniqueName="7" name="price" queryTableFieldId="6" dataDxfId="8"/>
-    <tableColumn id="8" uniqueName="8" name="advance" queryTableFieldId="7" dataDxfId="7"/>
-    <tableColumn id="9" uniqueName="9" name="royalty" queryTableFieldId="8" dataDxfId="6"/>
-    <tableColumn id="10" uniqueName="10" name="ytd_sales" queryTableFieldId="9" dataDxfId="5"/>
-    <tableColumn id="11" uniqueName="11" name="notes" queryTableFieldId="10" dataDxfId="4"/>
-    <tableColumn id="12" uniqueName="12" name="pubdate" queryTableFieldId="11" dataDxfId="3"/>
-    <tableColumn id="13" uniqueName="13" name="pub_id" queryTableFieldId="12" dataDxfId="2">
+    <tableColumn id="3" uniqueName="3" name="title_id" queryTableFieldId="2" dataDxfId="18"/>
+    <tableColumn id="4" uniqueName="4" name="title" queryTableFieldId="3" dataDxfId="17"/>
+    <tableColumn id="5" uniqueName="5" name="type" queryTableFieldId="4" dataDxfId="16"/>
+    <tableColumn id="6" uniqueName="6" name="pub_idLU" queryTableFieldId="5" dataDxfId="15"/>
+    <tableColumn id="7" uniqueName="7" name="price" queryTableFieldId="6" dataDxfId="14"/>
+    <tableColumn id="8" uniqueName="8" name="advance" queryTableFieldId="7" dataDxfId="13"/>
+    <tableColumn id="9" uniqueName="9" name="royalty" queryTableFieldId="8" dataDxfId="12"/>
+    <tableColumn id="10" uniqueName="10" name="ytd_sales" queryTableFieldId="9" dataDxfId="11"/>
+    <tableColumn id="11" uniqueName="11" name="notes" queryTableFieldId="10" dataDxfId="10"/>
+    <tableColumn id="12" uniqueName="12" name="pubdate" queryTableFieldId="11" dataDxfId="9"/>
+    <tableColumn id="13" uniqueName="13" name="pub_id" queryTableFieldId="12" dataDxfId="8">
       <calculatedColumnFormula>IF(Tabelle_ExterneDaten_19[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_19[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3378,7 +3374,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3388,20 +3384,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
-    <col min="2" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -4477,7 +4474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6207,7 +6206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7726,10 +7727,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7961,6 +7962,20 @@
         <v>100</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D16" s="2">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7973,7 +7988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>